<commit_message>
Added more rules and updated rules
</commit_message>
<xml_diff>
--- a/src/rule-files/CheckoutRules.xlsx
+++ b/src/rule-files/CheckoutRules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debojitroy/SomethingMeaningful/trool-checkout-discount-engine/src/rule-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{614AB263-D5FE-BA43-95F4-50776B2FEEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4556002E-985F-C147-9059-8A31FEF924D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{AF94D777-09A2-EE4F-A268-E8ED9A8D57E8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Condition</t>
   </si>
@@ -66,12 +66,48 @@
   <si>
     <t>New User - Flat 20% Discount</t>
   </si>
+  <si>
+    <t>Existing User - Order Value &gt; 1000</t>
+  </si>
+  <si>
+    <t>totalBeforeDiscount &gt;= $param</t>
+  </si>
+  <si>
+    <t>WelcomeBack Coupon</t>
+  </si>
+  <si>
+    <t>coupon == $param</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Import: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Coupons</t>
+    </r>
+  </si>
+  <si>
+    <t>WELCOMEBACK</t>
+  </si>
+  <si>
+    <t>“WELCOMEBACK”</t>
+  </si>
+  <si>
+    <t>Coupons.WELCOMEBACK</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,8 +121,19 @@
       <color theme="1"/>
       <name val="Liberation Sans"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +152,12 @@
         <bgColor rgb="FFFFE5CA"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBCE4E5"/>
+        <bgColor rgb="FFBCE4E5"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -198,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -209,6 +262,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,84 +580,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5461236A-7004-4940-BDCB-6DA5252B2DC9}">
-  <dimension ref="A2:C11"/>
+  <dimension ref="A2:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="35.83203125" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="4"/>
+      <c r="C5" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="11"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4"/>
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>